<commit_message>
Create/edit/delete for admins/experts only
</commit_message>
<xml_diff>
--- a/docs/use_cases_shanoir_ng.xlsx
+++ b/docs/use_cases_shanoir_ng.xlsx
@@ -741,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -763,7 +763,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">

</xml_diff>